<commit_message>
agrega el v-else del skeleton
</commit_message>
<xml_diff>
--- a/help-script/inputs/24_09_24.xlsx
+++ b/help-script/inputs/24_09_24.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="336">
   <si>
     <t xml:space="preserve">email </t>
   </si>
@@ -1036,7 +1036,7 @@
     <t>subscribedEventsId</t>
   </si>
   <si>
-    <t>4Ms88Hw9i3okcTHI7AV6</t>
+    <t>["4Ms88Hw9i3okcTHI7AV6"]</t>
   </si>
   <si>
     <t>Únete a la comunidad whatsapp del *concierto en el colegio Santa Úrsula* para que te enteres de todas las novedades.</t>
@@ -8525,8 +8525,8 @@
         <v>Avendaño</v>
       </c>
       <c r="D2" s="29" t="str">
-        <f>'Hoja 1'!F2</f>
-        <v>9 4261 6164</v>
+        <f>"+56"&amp;'Hoja 1'!F2</f>
+        <v>+569 4261 6164</v>
       </c>
       <c r="E2" s="29">
         <f>'Hoja 1'!E2</f>
@@ -8554,8 +8554,8 @@
         <v>Marín</v>
       </c>
       <c r="D3" s="29" t="str">
-        <f>'Hoja 1'!F3</f>
-        <v>9 8294 6322</v>
+        <f>"+56"&amp;'Hoja 1'!F3</f>
+        <v>+569 8294 6322</v>
       </c>
       <c r="E3" s="29">
         <f>'Hoja 1'!E3</f>
@@ -8583,8 +8583,8 @@
         <v>Von Appen</v>
       </c>
       <c r="D4" s="29" t="str">
-        <f>'Hoja 1'!F4</f>
-        <v>9 9744 6511</v>
+        <f>"+56"&amp;'Hoja 1'!F4</f>
+        <v>+569 9744 6511</v>
       </c>
       <c r="E4" s="29">
         <f>'Hoja 1'!E4</f>
@@ -8612,8 +8612,8 @@
         <v>Lagos</v>
       </c>
       <c r="D5" s="29" t="str">
-        <f>'Hoja 1'!F5</f>
-        <v>9 9846 1998</v>
+        <f>"+56"&amp;'Hoja 1'!F5</f>
+        <v>+569 9846 1998</v>
       </c>
       <c r="E5" s="29">
         <f>'Hoja 1'!E5</f>
@@ -8641,8 +8641,8 @@
         <v>Garcés</v>
       </c>
       <c r="D6" s="29" t="str">
-        <f>'Hoja 1'!F6</f>
-        <v>9 5226 5343</v>
+        <f>"+56"&amp;'Hoja 1'!F6</f>
+        <v>+569 5226 5343</v>
       </c>
       <c r="E6" s="29">
         <f>'Hoja 1'!E6</f>
@@ -8670,8 +8670,8 @@
         <v>Ebensperger</v>
       </c>
       <c r="D7" s="29" t="str">
-        <f>'Hoja 1'!F7</f>
-        <v>9 6640 8787</v>
+        <f>"+56"&amp;'Hoja 1'!F7</f>
+        <v>+569 6640 8787</v>
       </c>
       <c r="E7" s="29">
         <f>'Hoja 1'!E7</f>
@@ -8699,8 +8699,8 @@
         <v>Valdes</v>
       </c>
       <c r="D8" s="29" t="str">
-        <f>'Hoja 1'!F8</f>
-        <v>9 8501 2198</v>
+        <f>"+56"&amp;'Hoja 1'!F8</f>
+        <v>+569 8501 2198</v>
       </c>
       <c r="E8" s="29">
         <f>'Hoja 1'!E8</f>
@@ -8728,8 +8728,8 @@
         <v>Germain</v>
       </c>
       <c r="D9" s="29" t="str">
-        <f>'Hoja 1'!F9</f>
-        <v>9 9579 7158</v>
+        <f>"+56"&amp;'Hoja 1'!F9</f>
+        <v>+569 9579 7158</v>
       </c>
       <c r="E9" s="29">
         <f>'Hoja 1'!E9</f>
@@ -8757,8 +8757,8 @@
         <v>Lagos</v>
       </c>
       <c r="D10" s="29" t="str">
-        <f>'Hoja 1'!F10</f>
-        <v>9 9825 8380</v>
+        <f>"+56"&amp;'Hoja 1'!F10</f>
+        <v>+569 9825 8380</v>
       </c>
       <c r="E10" s="29">
         <f>'Hoja 1'!E10</f>
@@ -8786,8 +8786,8 @@
         <v>Cherniavsky</v>
       </c>
       <c r="D11" s="29" t="str">
-        <f>'Hoja 1'!F11</f>
-        <v>9 8288 1756</v>
+        <f>"+56"&amp;'Hoja 1'!F11</f>
+        <v>+569 8288 1756</v>
       </c>
       <c r="E11" s="29">
         <f>'Hoja 1'!E11</f>
@@ -8815,8 +8815,8 @@
         <v>Gomez</v>
       </c>
       <c r="D12" s="29" t="str">
-        <f>'Hoja 1'!F12</f>
-        <v>9 6326 0713</v>
+        <f>"+56"&amp;'Hoja 1'!F12</f>
+        <v>+569 6326 0713</v>
       </c>
       <c r="E12" s="29">
         <f>'Hoja 1'!E12</f>
@@ -8844,8 +8844,8 @@
         <v>Schultz</v>
       </c>
       <c r="D13" s="29" t="str">
-        <f>'Hoja 1'!F13</f>
-        <v>9 8199 8599</v>
+        <f>"+56"&amp;'Hoja 1'!F13</f>
+        <v>+569 8199 8599</v>
       </c>
       <c r="E13" s="29">
         <f>'Hoja 1'!E13</f>
@@ -8873,8 +8873,8 @@
         <v>Ovalle</v>
       </c>
       <c r="D14" s="29" t="str">
-        <f>'Hoja 1'!F14</f>
-        <v>9 9336 8303</v>
+        <f>"+56"&amp;'Hoja 1'!F14</f>
+        <v>+569 9336 8303</v>
       </c>
       <c r="E14" s="29">
         <f>'Hoja 1'!E14</f>
@@ -8902,8 +8902,8 @@
         <v>Hederra</v>
       </c>
       <c r="D15" s="29" t="str">
-        <f>'Hoja 1'!F15</f>
-        <v>9 8237 2510</v>
+        <f>"+56"&amp;'Hoja 1'!F15</f>
+        <v>+569 8237 2510</v>
       </c>
       <c r="E15" s="29">
         <f>'Hoja 1'!E15</f>
@@ -8931,8 +8931,8 @@
         <v>Lagos</v>
       </c>
       <c r="D16" s="29" t="str">
-        <f>'Hoja 1'!F16</f>
-        <v>9 9753 8124</v>
+        <f>"+56"&amp;'Hoja 1'!F16</f>
+        <v>+569 9753 8124</v>
       </c>
       <c r="E16" s="29">
         <f>'Hoja 1'!E16</f>
@@ -8960,8 +8960,8 @@
         <v>Bier</v>
       </c>
       <c r="D17" s="29" t="str">
-        <f>'Hoja 1'!F17</f>
-        <v>9 9779 6429</v>
+        <f>"+56"&amp;'Hoja 1'!F17</f>
+        <v>+569 9779 6429</v>
       </c>
       <c r="E17" s="29">
         <f>'Hoja 1'!E17</f>
@@ -8989,8 +8989,8 @@
         <v>Faille</v>
       </c>
       <c r="D18" s="29" t="str">
-        <f>'Hoja 1'!F18</f>
-        <v>9 9886 0126</v>
+        <f>"+56"&amp;'Hoja 1'!F18</f>
+        <v>+569 9886 0126</v>
       </c>
       <c r="E18" s="29">
         <f>'Hoja 1'!E18</f>
@@ -9018,8 +9018,8 @@
         <v>Larrain Queiroz</v>
       </c>
       <c r="D19" s="29" t="str">
-        <f>'Hoja 1'!F19</f>
-        <v>9 7609 7255</v>
+        <f>"+56"&amp;'Hoja 1'!F19</f>
+        <v>+569 7609 7255</v>
       </c>
       <c r="E19" s="29">
         <f>'Hoja 1'!E19</f>
@@ -9047,8 +9047,8 @@
         <v>Roa</v>
       </c>
       <c r="D20" s="29" t="str">
-        <f>'Hoja 1'!F20</f>
-        <v>9 9214 4516</v>
+        <f>"+56"&amp;'Hoja 1'!F20</f>
+        <v>+569 9214 4516</v>
       </c>
       <c r="E20" s="29">
         <f>'Hoja 1'!E20</f>
@@ -9076,8 +9076,8 @@
         <v>Riesco Vicuña</v>
       </c>
       <c r="D21" s="29" t="str">
-        <f>'Hoja 1'!F21</f>
-        <v>9 9020 8985</v>
+        <f>"+56"&amp;'Hoja 1'!F21</f>
+        <v>+569 9020 8985</v>
       </c>
       <c r="E21" s="29">
         <f>'Hoja 1'!E21</f>
@@ -9105,8 +9105,8 @@
         <v>Galleguillos</v>
       </c>
       <c r="D22" s="29" t="str">
-        <f>'Hoja 1'!F22</f>
-        <v>9 4262 3063</v>
+        <f>"+56"&amp;'Hoja 1'!F22</f>
+        <v>+569 4262 3063</v>
       </c>
       <c r="E22" s="29">
         <f>'Hoja 1'!E22</f>
@@ -9134,8 +9134,8 @@
         <v>Garcia Huidobro </v>
       </c>
       <c r="D23" s="29" t="str">
-        <f>'Hoja 1'!F23</f>
-        <v>9 9822 7413</v>
+        <f>"+56"&amp;'Hoja 1'!F23</f>
+        <v>+569 9822 7413</v>
       </c>
       <c r="E23" s="29">
         <f>'Hoja 1'!E23</f>
@@ -9163,8 +9163,8 @@
         <v>Müller</v>
       </c>
       <c r="D24" s="29" t="str">
-        <f>'Hoja 1'!F24</f>
-        <v>9 6587 1743</v>
+        <f>"+56"&amp;'Hoja 1'!F24</f>
+        <v>+569 6587 1743</v>
       </c>
       <c r="E24" s="29">
         <f>'Hoja 1'!E24</f>
@@ -9192,8 +9192,8 @@
         <v>Jeldres</v>
       </c>
       <c r="D25" s="29" t="str">
-        <f>'Hoja 1'!F25</f>
-        <v>9 3456 9320</v>
+        <f>"+56"&amp;'Hoja 1'!F25</f>
+        <v>+569 3456 9320</v>
       </c>
       <c r="E25" s="29">
         <f>'Hoja 1'!E25</f>
@@ -9221,8 +9221,8 @@
         <v>Nuñez Sánchez</v>
       </c>
       <c r="D26" s="29" t="str">
-        <f>'Hoja 1'!F26</f>
-        <v>9 9894 5348</v>
+        <f>"+56"&amp;'Hoja 1'!F26</f>
+        <v>+569 9894 5348</v>
       </c>
       <c r="E26" s="29">
         <f>'Hoja 1'!E26</f>
@@ -9250,8 +9250,8 @@
         <v>Romo Figueroa</v>
       </c>
       <c r="D27" s="29" t="str">
-        <f>'Hoja 1'!F27</f>
-        <v>9 9732 5679</v>
+        <f>"+56"&amp;'Hoja 1'!F27</f>
+        <v>+569 9732 5679</v>
       </c>
       <c r="E27" s="29">
         <f>'Hoja 1'!E27</f>
@@ -9279,8 +9279,8 @@
         <v>Pumpin</v>
       </c>
       <c r="D28" s="29" t="str">
-        <f>'Hoja 1'!F28</f>
-        <v>9 9840 4320</v>
+        <f>"+56"&amp;'Hoja 1'!F28</f>
+        <v>+569 9840 4320</v>
       </c>
       <c r="E28" s="29">
         <f>'Hoja 1'!E28</f>
@@ -9308,8 +9308,8 @@
         <v>Angerstein</v>
       </c>
       <c r="D29" s="29" t="str">
-        <f>'Hoja 1'!F29</f>
-        <v>9 8829 8674</v>
+        <f>"+56"&amp;'Hoja 1'!F29</f>
+        <v>+569 8829 8674</v>
       </c>
       <c r="E29" s="29">
         <f>'Hoja 1'!E29</f>
@@ -9337,8 +9337,8 @@
         <v>OShea</v>
       </c>
       <c r="D30" s="29" t="str">
-        <f>'Hoja 1'!F30</f>
-        <v>9 9863 5607</v>
+        <f>"+56"&amp;'Hoja 1'!F30</f>
+        <v>+569 9863 5607</v>
       </c>
       <c r="E30" s="29">
         <f>'Hoja 1'!E30</f>
@@ -9366,8 +9366,8 @@
         <v>Salazar Bolaño</v>
       </c>
       <c r="D31" s="29" t="str">
-        <f>'Hoja 1'!F31</f>
-        <v>9 9863 3818</v>
+        <f>"+56"&amp;'Hoja 1'!F31</f>
+        <v>+569 9863 3818</v>
       </c>
       <c r="E31" s="29">
         <f>'Hoja 1'!E31</f>
@@ -9395,8 +9395,8 @@
         <v>Yon</v>
       </c>
       <c r="D32" s="29" t="str">
-        <f>'Hoja 1'!F32</f>
-        <v>9 9758 8221</v>
+        <f>"+56"&amp;'Hoja 1'!F32</f>
+        <v>+569 9758 8221</v>
       </c>
       <c r="E32" s="29">
         <f>'Hoja 1'!E32</f>
@@ -9424,8 +9424,8 @@
         <v>Valdes</v>
       </c>
       <c r="D33" s="29" t="str">
-        <f>'Hoja 1'!F33</f>
-        <v>9 7758 1698</v>
+        <f>"+56"&amp;'Hoja 1'!F33</f>
+        <v>+569 7758 1698</v>
       </c>
       <c r="E33" s="29">
         <f>'Hoja 1'!E33</f>
@@ -9453,8 +9453,8 @@
         <v>Barros</v>
       </c>
       <c r="D34" s="29" t="str">
-        <f>'Hoja 1'!F34</f>
-        <v>9 8429 9534</v>
+        <f>"+56"&amp;'Hoja 1'!F34</f>
+        <v>+569 8429 9534</v>
       </c>
       <c r="E34" s="29">
         <f>'Hoja 1'!E34</f>
@@ -9482,8 +9482,8 @@
         <v>Delucchi</v>
       </c>
       <c r="D35" s="29" t="str">
-        <f>'Hoja 1'!F35</f>
-        <v>9 5671 0413</v>
+        <f>"+56"&amp;'Hoja 1'!F35</f>
+        <v>+569 5671 0413</v>
       </c>
       <c r="E35" s="29">
         <f>'Hoja 1'!E35</f>
@@ -9511,8 +9511,8 @@
         <v>Kast</v>
       </c>
       <c r="D36" s="29" t="str">
-        <f>'Hoja 1'!F36</f>
-        <v>9 6249 2200</v>
+        <f>"+56"&amp;'Hoja 1'!F36</f>
+        <v>+569 6249 2200</v>
       </c>
       <c r="E36" s="29">
         <f>'Hoja 1'!E36</f>
@@ -9540,8 +9540,8 @@
         <v>Herrera</v>
       </c>
       <c r="D37" s="29" t="str">
-        <f>'Hoja 1'!F37</f>
-        <v>9 9342 1609</v>
+        <f>"+56"&amp;'Hoja 1'!F37</f>
+        <v>+569 9342 1609</v>
       </c>
       <c r="E37" s="29">
         <f>'Hoja 1'!E37</f>
@@ -9569,8 +9569,8 @@
         <v>Unterhofer</v>
       </c>
       <c r="D38" s="29" t="str">
-        <f>'Hoja 1'!F38</f>
-        <v>9 8239 2635</v>
+        <f>"+56"&amp;'Hoja 1'!F38</f>
+        <v>+569 8239 2635</v>
       </c>
       <c r="E38" s="29">
         <f>'Hoja 1'!E38</f>
@@ -9598,8 +9598,8 @@
         <v>Briones</v>
       </c>
       <c r="D39" s="29" t="str">
-        <f>'Hoja 1'!F39</f>
-        <v>9 9289 7467</v>
+        <f>"+56"&amp;'Hoja 1'!F39</f>
+        <v>+569 9289 7467</v>
       </c>
       <c r="E39" s="29">
         <f>'Hoja 1'!E39</f>
@@ -9627,8 +9627,8 @@
         <v>Branth</v>
       </c>
       <c r="D40" s="29" t="str">
-        <f>'Hoja 1'!F40</f>
-        <v>9 9359 1841</v>
+        <f>"+56"&amp;'Hoja 1'!F40</f>
+        <v>+569 9359 1841</v>
       </c>
       <c r="E40" s="29">
         <f>'Hoja 1'!E40</f>
@@ -9656,8 +9656,8 @@
         <v>Valverde</v>
       </c>
       <c r="D41" s="29" t="str">
-        <f>'Hoja 1'!F41</f>
-        <v>9 8217 4162</v>
+        <f>"+56"&amp;'Hoja 1'!F41</f>
+        <v>+569 8217 4162</v>
       </c>
       <c r="E41" s="29">
         <f>'Hoja 1'!E41</f>
@@ -9685,8 +9685,8 @@
         <v>Gómez O.</v>
       </c>
       <c r="D42" s="29" t="str">
-        <f>'Hoja 1'!F42</f>
-        <v>9 9643 3015</v>
+        <f>"+56"&amp;'Hoja 1'!F42</f>
+        <v>+569 9643 3015</v>
       </c>
       <c r="E42" s="29">
         <f>'Hoja 1'!E42</f>
@@ -9714,8 +9714,8 @@
         <v>Toro</v>
       </c>
       <c r="D43" s="29" t="str">
-        <f>'Hoja 1'!F43</f>
-        <v>9 9239 5445</v>
+        <f>"+56"&amp;'Hoja 1'!F43</f>
+        <v>+569 9239 5445</v>
       </c>
       <c r="E43" s="29">
         <f>'Hoja 1'!E43</f>
@@ -9743,8 +9743,8 @@
         <v>Fonck</v>
       </c>
       <c r="D44" s="29" t="str">
-        <f>'Hoja 1'!F44</f>
-        <v>9 7668 8724</v>
+        <f>"+56"&amp;'Hoja 1'!F44</f>
+        <v>+569 7668 8724</v>
       </c>
       <c r="E44" s="29">
         <f>'Hoja 1'!E44</f>
@@ -9772,8 +9772,8 @@
         <v>Bascuñán</v>
       </c>
       <c r="D45" s="29" t="str">
-        <f>'Hoja 1'!F45</f>
-        <v>9 8159 8421</v>
+        <f>"+56"&amp;'Hoja 1'!F45</f>
+        <v>+569 8159 8421</v>
       </c>
       <c r="E45" s="29">
         <f>'Hoja 1'!E45</f>
@@ -9801,8 +9801,8 @@
         <v>Scherholz</v>
       </c>
       <c r="D46" s="29" t="str">
-        <f>'Hoja 1'!F46</f>
-        <v>9 9382 0869</v>
+        <f>"+56"&amp;'Hoja 1'!F46</f>
+        <v>+569 9382 0869</v>
       </c>
       <c r="E46" s="29">
         <f>'Hoja 1'!E46</f>
@@ -9830,8 +9830,8 @@
         <v>Sieverson</v>
       </c>
       <c r="D47" s="29" t="str">
-        <f>'Hoja 1'!F47</f>
-        <v>9 8575 7457</v>
+        <f>"+56"&amp;'Hoja 1'!F47</f>
+        <v>+569 8575 7457</v>
       </c>
       <c r="E47" s="29">
         <f>'Hoja 1'!E47</f>
@@ -9859,8 +9859,8 @@
         <v>Sutter</v>
       </c>
       <c r="D48" s="29" t="str">
-        <f>'Hoja 1'!F48</f>
-        <v>9 9541 0287</v>
+        <f>"+56"&amp;'Hoja 1'!F48</f>
+        <v>+569 9541 0287</v>
       </c>
       <c r="E48" s="29">
         <f>'Hoja 1'!E48</f>
@@ -9888,8 +9888,8 @@
         <v>Tonkin</v>
       </c>
       <c r="D49" s="29" t="str">
-        <f>'Hoja 1'!F49</f>
-        <v>9 9218 6182</v>
+        <f>"+56"&amp;'Hoja 1'!F49</f>
+        <v>+569 9218 6182</v>
       </c>
       <c r="E49" s="29">
         <f>'Hoja 1'!E49</f>
@@ -9917,8 +9917,8 @@
         <v>Prado</v>
       </c>
       <c r="D50" s="29" t="str">
-        <f>'Hoja 1'!F50</f>
-        <v>9 8808 0831</v>
+        <f>"+56"&amp;'Hoja 1'!F50</f>
+        <v>+569 8808 0831</v>
       </c>
       <c r="E50" s="29">
         <f>'Hoja 1'!E50</f>
@@ -9946,8 +9946,8 @@
         <v>Castillo</v>
       </c>
       <c r="D51" s="29" t="str">
-        <f>'Hoja 1'!F51</f>
-        <v>9 9318 8388</v>
+        <f>"+56"&amp;'Hoja 1'!F51</f>
+        <v>+569 9318 8388</v>
       </c>
       <c r="E51" s="29">
         <f>'Hoja 1'!E51</f>
@@ -9975,8 +9975,8 @@
         <v>Torrealba</v>
       </c>
       <c r="D52" s="29" t="str">
-        <f>'Hoja 1'!F52</f>
-        <v>9 9018 4609</v>
+        <f>"+56"&amp;'Hoja 1'!F52</f>
+        <v>+569 9018 4609</v>
       </c>
       <c r="E52" s="29">
         <f>'Hoja 1'!E52</f>
@@ -10004,8 +10004,8 @@
         <v>Pozo</v>
       </c>
       <c r="D53" s="29" t="str">
-        <f>'Hoja 1'!F53</f>
-        <v>9 9146 0608</v>
+        <f>"+56"&amp;'Hoja 1'!F53</f>
+        <v>+569 9146 0608</v>
       </c>
       <c r="E53" s="29">
         <f>'Hoja 1'!E53</f>
@@ -10033,8 +10033,8 @@
         <v>Dominguez R-T</v>
       </c>
       <c r="D54" s="29" t="str">
-        <f>'Hoja 1'!F54</f>
-        <v>9 8828 7562</v>
+        <f>"+56"&amp;'Hoja 1'!F54</f>
+        <v>+569 8828 7562</v>
       </c>
       <c r="E54" s="29">
         <f>'Hoja 1'!E54</f>
@@ -10062,8 +10062,8 @@
         <v>Toro Anastassiou</v>
       </c>
       <c r="D55" s="29" t="str">
-        <f>'Hoja 1'!F55</f>
-        <v>9 9682 8078</v>
+        <f>"+56"&amp;'Hoja 1'!F55</f>
+        <v>+569 9682 8078</v>
       </c>
       <c r="E55" s="29">
         <f>'Hoja 1'!E55</f>
@@ -10091,8 +10091,8 @@
         <v>Quiroga Newbery</v>
       </c>
       <c r="D56" s="29" t="str">
-        <f>'Hoja 1'!F56</f>
-        <v>9 7440 2072</v>
+        <f>"+56"&amp;'Hoja 1'!F56</f>
+        <v>+569 7440 2072</v>
       </c>
       <c r="E56" s="29">
         <f>'Hoja 1'!E56</f>
@@ -10120,8 +10120,8 @@
         <v>Toro Labbé</v>
       </c>
       <c r="D57" s="29" t="str">
-        <f>'Hoja 1'!F57</f>
-        <v>9 9730 7516</v>
+        <f>"+56"&amp;'Hoja 1'!F57</f>
+        <v>+569 9730 7516</v>
       </c>
       <c r="E57" s="29">
         <f>'Hoja 1'!E57</f>
@@ -10149,8 +10149,8 @@
         <v>Bianch</v>
       </c>
       <c r="D58" s="29" t="str">
-        <f>'Hoja 1'!F58</f>
-        <v>9 9078 8471</v>
+        <f>"+56"&amp;'Hoja 1'!F58</f>
+        <v>+569 9078 8471</v>
       </c>
       <c r="E58" s="29">
         <f>'Hoja 1'!E58</f>
@@ -10178,8 +10178,8 @@
         <v>Ferrer</v>
       </c>
       <c r="D59" s="29" t="str">
-        <f>'Hoja 1'!F59</f>
-        <v>9 9079 3214</v>
+        <f>"+56"&amp;'Hoja 1'!F59</f>
+        <v>+569 9079 3214</v>
       </c>
       <c r="E59" s="29">
         <f>'Hoja 1'!E59</f>
@@ -10207,8 +10207,8 @@
         <v>Ferrer</v>
       </c>
       <c r="D60" s="29" t="str">
-        <f>'Hoja 1'!F60</f>
-        <v>9 9750 3114</v>
+        <f>"+56"&amp;'Hoja 1'!F60</f>
+        <v>+569 9750 3114</v>
       </c>
       <c r="E60" s="29">
         <f>'Hoja 1'!E60</f>
@@ -10236,8 +10236,8 @@
         <v>Redard</v>
       </c>
       <c r="D61" s="29" t="str">
-        <f>'Hoja 1'!F61</f>
-        <v>9 8904 8448</v>
+        <f>"+56"&amp;'Hoja 1'!F61</f>
+        <v>+569 8904 8448</v>
       </c>
       <c r="E61" s="29">
         <f>'Hoja 1'!E61</f>
@@ -10265,8 +10265,8 @@
         <v>Vergara</v>
       </c>
       <c r="D62" s="29" t="str">
-        <f>'Hoja 1'!F62</f>
-        <v>9 7307 2401</v>
+        <f>"+56"&amp;'Hoja 1'!F62</f>
+        <v>+569 7307 2401</v>
       </c>
       <c r="E62" s="29">
         <f>'Hoja 1'!E62</f>
@@ -10294,8 +10294,8 @@
         <v>Recher</v>
       </c>
       <c r="D63" s="29" t="str">
-        <f>'Hoja 1'!F63</f>
-        <v>9 7700 8293</v>
+        <f>"+56"&amp;'Hoja 1'!F63</f>
+        <v>+569 7700 8293</v>
       </c>
       <c r="E63" s="29">
         <f>'Hoja 1'!E63</f>
@@ -10323,8 +10323,8 @@
         <v>Yuraszeck</v>
       </c>
       <c r="D64" s="29" t="str">
-        <f>'Hoja 1'!F64</f>
-        <v>9 9824 8737</v>
+        <f>"+56"&amp;'Hoja 1'!F64</f>
+        <v>+569 9824 8737</v>
       </c>
       <c r="E64" s="29">
         <f>'Hoja 1'!E64</f>
@@ -10352,8 +10352,8 @@
         <v>Urrejola</v>
       </c>
       <c r="D65" s="29" t="str">
-        <f>'Hoja 1'!F65</f>
-        <v>9 9467 6669</v>
+        <f>"+56"&amp;'Hoja 1'!F65</f>
+        <v>+569 9467 6669</v>
       </c>
       <c r="E65" s="29">
         <f>'Hoja 1'!E65</f>
@@ -10381,8 +10381,8 @@
         <v>Recher</v>
       </c>
       <c r="D66" s="29" t="str">
-        <f>'Hoja 1'!F66</f>
-        <v>9 9341 9665</v>
+        <f>"+56"&amp;'Hoja 1'!F66</f>
+        <v>+569 9341 9665</v>
       </c>
       <c r="E66" s="29">
         <f>'Hoja 1'!E66</f>
@@ -10410,8 +10410,8 @@
         <v>Donoso Cuevas</v>
       </c>
       <c r="D67" s="29" t="str">
-        <f>'Hoja 1'!F67</f>
-        <v>9 7400 6532</v>
+        <f>"+56"&amp;'Hoja 1'!F67</f>
+        <v>+569 7400 6532</v>
       </c>
       <c r="E67" s="29">
         <f>'Hoja 1'!E67</f>
@@ -10439,8 +10439,8 @@
         <v>Varas</v>
       </c>
       <c r="D68" s="29" t="str">
-        <f>'Hoja 1'!F68</f>
-        <v>9 9299 1714</v>
+        <f>"+56"&amp;'Hoja 1'!F68</f>
+        <v>+569 9299 1714</v>
       </c>
       <c r="E68" s="29">
         <f>'Hoja 1'!E68</f>
@@ -10468,8 +10468,8 @@
         <v>Izquierdo</v>
       </c>
       <c r="D69" s="29" t="str">
-        <f>'Hoja 1'!F69</f>
-        <v>9 9482 9661</v>
+        <f>"+56"&amp;'Hoja 1'!F69</f>
+        <v>+569 9482 9661</v>
       </c>
       <c r="E69" s="29">
         <f>'Hoja 1'!E69</f>
@@ -10497,8 +10497,8 @@
         <v>Grez</v>
       </c>
       <c r="D70" s="29" t="str">
-        <f>'Hoja 1'!F70</f>
-        <v>9 8288 1588</v>
+        <f>"+56"&amp;'Hoja 1'!F70</f>
+        <v>+569 8288 1588</v>
       </c>
       <c r="E70" s="29">
         <f>'Hoja 1'!E70</f>
@@ -10526,8 +10526,8 @@
         <v>Gajardo</v>
       </c>
       <c r="D71" s="29" t="str">
-        <f>'Hoja 1'!F71</f>
-        <v>9 9494 9321</v>
+        <f>"+56"&amp;'Hoja 1'!F71</f>
+        <v>+569 9494 9321</v>
       </c>
       <c r="E71" s="29">
         <f>'Hoja 1'!E71</f>
@@ -10555,8 +10555,8 @@
         <v/>
       </c>
       <c r="D72" s="29" t="str">
-        <f>'Hoja 1'!F72</f>
-        <v/>
+        <f>"+56"&amp;'Hoja 1'!F72</f>
+        <v>+56</v>
       </c>
       <c r="E72" s="29" t="str">
         <f>'Hoja 1'!E72</f>
@@ -10584,8 +10584,8 @@
         <v/>
       </c>
       <c r="D73" s="29" t="str">
-        <f>'Hoja 1'!F73</f>
-        <v/>
+        <f>"+56"&amp;'Hoja 1'!F73</f>
+        <v>+56</v>
       </c>
       <c r="E73" s="29" t="str">
         <f>'Hoja 1'!E73</f>
@@ -10613,8 +10613,8 @@
         <v/>
       </c>
       <c r="D74" s="29" t="str">
-        <f>'Hoja 1'!F74</f>
-        <v/>
+        <f>"+56"&amp;'Hoja 1'!F74</f>
+        <v>+56</v>
       </c>
       <c r="E74" s="29" t="str">
         <f>'Hoja 1'!E74</f>
@@ -10642,8 +10642,8 @@
         <v/>
       </c>
       <c r="D75" s="29" t="str">
-        <f>'Hoja 1'!F75</f>
-        <v/>
+        <f>"+56"&amp;'Hoja 1'!F75</f>
+        <v>+56</v>
       </c>
       <c r="E75" s="29" t="str">
         <f>'Hoja 1'!E75</f>
@@ -10671,8 +10671,8 @@
         <v/>
       </c>
       <c r="D76" s="29" t="str">
-        <f>'Hoja 1'!F76</f>
-        <v/>
+        <f>"+56"&amp;'Hoja 1'!F76</f>
+        <v>+56</v>
       </c>
       <c r="E76" s="29" t="str">
         <f>'Hoja 1'!E76</f>
@@ -10700,8 +10700,8 @@
         <v/>
       </c>
       <c r="D77" s="29" t="str">
-        <f>'Hoja 1'!F77</f>
-        <v/>
+        <f>"+56"&amp;'Hoja 1'!F77</f>
+        <v>+56</v>
       </c>
       <c r="E77" s="29" t="str">
         <f>'Hoja 1'!E77</f>
@@ -10729,8 +10729,8 @@
         <v/>
       </c>
       <c r="D78" s="29" t="str">
-        <f>'Hoja 1'!F78</f>
-        <v/>
+        <f>"+56"&amp;'Hoja 1'!F78</f>
+        <v>+56</v>
       </c>
       <c r="E78" s="29" t="str">
         <f>'Hoja 1'!E78</f>
@@ -10758,8 +10758,8 @@
         <v/>
       </c>
       <c r="D79" s="29" t="str">
-        <f>'Hoja 1'!F79</f>
-        <v/>
+        <f>"+56"&amp;'Hoja 1'!F79</f>
+        <v>+56</v>
       </c>
       <c r="E79" s="29" t="str">
         <f>'Hoja 1'!E79</f>
@@ -10787,8 +10787,8 @@
         <v/>
       </c>
       <c r="D80" s="29" t="str">
-        <f>'Hoja 1'!F80</f>
-        <v/>
+        <f>"+56"&amp;'Hoja 1'!F80</f>
+        <v>+56</v>
       </c>
       <c r="E80" s="29" t="str">
         <f>'Hoja 1'!E80</f>
@@ -10816,8 +10816,8 @@
         <v/>
       </c>
       <c r="D81" s="29" t="str">
-        <f>'Hoja 1'!F81</f>
-        <v/>
+        <f>"+56"&amp;'Hoja 1'!F81</f>
+        <v>+56</v>
       </c>
       <c r="E81" s="29" t="str">
         <f>'Hoja 1'!E81</f>
@@ -10832,6 +10832,26 @@
       </c>
     </row>
     <row r="82">
+      <c r="A82" s="29" t="str">
+        <f>'Hoja 1'!B82</f>
+        <v/>
+      </c>
+      <c r="B82" s="29" t="str">
+        <f>'Hoja 1'!C82</f>
+        <v/>
+      </c>
+      <c r="C82" s="29" t="str">
+        <f>'Hoja 1'!D82</f>
+        <v/>
+      </c>
+      <c r="D82" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F82</f>
+        <v>+56</v>
+      </c>
+      <c r="E82" s="29" t="str">
+        <f>'Hoja 1'!E82</f>
+        <v/>
+      </c>
       <c r="F82" s="29" t="str">
         <f>'Hoja 1'!I82</f>
         <v/>
@@ -10841,6 +10861,26 @@
       </c>
     </row>
     <row r="83">
+      <c r="A83" s="29" t="str">
+        <f>'Hoja 1'!B83</f>
+        <v/>
+      </c>
+      <c r="B83" s="29" t="str">
+        <f>'Hoja 1'!C83</f>
+        <v/>
+      </c>
+      <c r="C83" s="29" t="str">
+        <f>'Hoja 1'!D83</f>
+        <v/>
+      </c>
+      <c r="D83" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F83</f>
+        <v>+56</v>
+      </c>
+      <c r="E83" s="29" t="str">
+        <f>'Hoja 1'!E83</f>
+        <v/>
+      </c>
       <c r="F83" s="29" t="str">
         <f>'Hoja 1'!I83</f>
         <v/>
@@ -10850,6 +10890,26 @@
       </c>
     </row>
     <row r="84">
+      <c r="A84" s="29" t="str">
+        <f>'Hoja 1'!B84</f>
+        <v/>
+      </c>
+      <c r="B84" s="29" t="str">
+        <f>'Hoja 1'!C84</f>
+        <v/>
+      </c>
+      <c r="C84" s="29" t="str">
+        <f>'Hoja 1'!D84</f>
+        <v/>
+      </c>
+      <c r="D84" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F84</f>
+        <v>+56</v>
+      </c>
+      <c r="E84" s="29" t="str">
+        <f>'Hoja 1'!E84</f>
+        <v/>
+      </c>
       <c r="F84" s="29" t="str">
         <f>'Hoja 1'!I84</f>
         <v/>
@@ -10859,232 +10919,1365 @@
       </c>
     </row>
     <row r="85">
+      <c r="A85" s="29" t="str">
+        <f>'Hoja 1'!B85</f>
+        <v/>
+      </c>
+      <c r="B85" s="29" t="str">
+        <f>'Hoja 1'!C85</f>
+        <v/>
+      </c>
+      <c r="C85" s="29" t="str">
+        <f>'Hoja 1'!D85</f>
+        <v/>
+      </c>
+      <c r="D85" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F85</f>
+        <v>+56</v>
+      </c>
+      <c r="E85" s="29" t="str">
+        <f>'Hoja 1'!E85</f>
+        <v/>
+      </c>
+      <c r="F85" s="29" t="str">
+        <f>'Hoja 1'!I85</f>
+        <v/>
+      </c>
       <c r="G85" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="86">
+      <c r="A86" s="29" t="str">
+        <f>'Hoja 1'!B86</f>
+        <v/>
+      </c>
+      <c r="B86" s="29" t="str">
+        <f>'Hoja 1'!C86</f>
+        <v/>
+      </c>
+      <c r="C86" s="29" t="str">
+        <f>'Hoja 1'!D86</f>
+        <v/>
+      </c>
+      <c r="D86" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F86</f>
+        <v>+56</v>
+      </c>
+      <c r="E86" s="29" t="str">
+        <f>'Hoja 1'!E86</f>
+        <v/>
+      </c>
+      <c r="F86" s="29" t="str">
+        <f>'Hoja 1'!I86</f>
+        <v/>
+      </c>
       <c r="G86" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="87">
+      <c r="A87" s="29" t="str">
+        <f>'Hoja 1'!B87</f>
+        <v/>
+      </c>
+      <c r="B87" s="29" t="str">
+        <f>'Hoja 1'!C87</f>
+        <v/>
+      </c>
+      <c r="C87" s="29" t="str">
+        <f>'Hoja 1'!D87</f>
+        <v/>
+      </c>
+      <c r="D87" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F87</f>
+        <v>+56</v>
+      </c>
+      <c r="E87" s="29" t="str">
+        <f>'Hoja 1'!E87</f>
+        <v/>
+      </c>
+      <c r="F87" s="29" t="str">
+        <f>'Hoja 1'!I87</f>
+        <v/>
+      </c>
       <c r="G87" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="88">
+      <c r="A88" s="29" t="str">
+        <f>'Hoja 1'!B88</f>
+        <v/>
+      </c>
+      <c r="B88" s="29" t="str">
+        <f>'Hoja 1'!C88</f>
+        <v/>
+      </c>
+      <c r="C88" s="29" t="str">
+        <f>'Hoja 1'!D88</f>
+        <v/>
+      </c>
+      <c r="D88" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F88</f>
+        <v>+56</v>
+      </c>
+      <c r="E88" s="29" t="str">
+        <f>'Hoja 1'!E88</f>
+        <v/>
+      </c>
+      <c r="F88" s="29" t="str">
+        <f>'Hoja 1'!I88</f>
+        <v/>
+      </c>
       <c r="G88" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="89">
+      <c r="A89" s="29" t="str">
+        <f>'Hoja 1'!B89</f>
+        <v/>
+      </c>
+      <c r="B89" s="29" t="str">
+        <f>'Hoja 1'!C89</f>
+        <v/>
+      </c>
+      <c r="C89" s="29" t="str">
+        <f>'Hoja 1'!D89</f>
+        <v/>
+      </c>
+      <c r="D89" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F89</f>
+        <v>+56</v>
+      </c>
+      <c r="E89" s="29" t="str">
+        <f>'Hoja 1'!E89</f>
+        <v/>
+      </c>
+      <c r="F89" s="29" t="str">
+        <f>'Hoja 1'!I89</f>
+        <v/>
+      </c>
       <c r="G89" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="90">
+      <c r="A90" s="29" t="str">
+        <f>'Hoja 1'!B90</f>
+        <v/>
+      </c>
+      <c r="B90" s="29" t="str">
+        <f>'Hoja 1'!C90</f>
+        <v/>
+      </c>
+      <c r="C90" s="29" t="str">
+        <f>'Hoja 1'!D90</f>
+        <v/>
+      </c>
+      <c r="D90" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F90</f>
+        <v>+56</v>
+      </c>
+      <c r="E90" s="29" t="str">
+        <f>'Hoja 1'!E90</f>
+        <v/>
+      </c>
+      <c r="F90" s="29" t="str">
+        <f>'Hoja 1'!I90</f>
+        <v/>
+      </c>
       <c r="G90" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="91">
+      <c r="A91" s="29" t="str">
+        <f>'Hoja 1'!B91</f>
+        <v/>
+      </c>
+      <c r="B91" s="29" t="str">
+        <f>'Hoja 1'!C91</f>
+        <v/>
+      </c>
+      <c r="C91" s="29" t="str">
+        <f>'Hoja 1'!D91</f>
+        <v/>
+      </c>
+      <c r="D91" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F91</f>
+        <v>+56</v>
+      </c>
+      <c r="E91" s="29" t="str">
+        <f>'Hoja 1'!E91</f>
+        <v/>
+      </c>
+      <c r="F91" s="29" t="str">
+        <f>'Hoja 1'!I91</f>
+        <v/>
+      </c>
       <c r="G91" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="92">
+      <c r="A92" s="29" t="str">
+        <f>'Hoja 1'!B92</f>
+        <v/>
+      </c>
+      <c r="B92" s="29" t="str">
+        <f>'Hoja 1'!C92</f>
+        <v/>
+      </c>
+      <c r="C92" s="29" t="str">
+        <f>'Hoja 1'!D92</f>
+        <v/>
+      </c>
+      <c r="D92" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F92</f>
+        <v>+56</v>
+      </c>
+      <c r="E92" s="29" t="str">
+        <f>'Hoja 1'!E92</f>
+        <v/>
+      </c>
+      <c r="F92" s="29" t="str">
+        <f>'Hoja 1'!I92</f>
+        <v/>
+      </c>
       <c r="G92" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="93">
+      <c r="A93" s="29" t="str">
+        <f>'Hoja 1'!B93</f>
+        <v/>
+      </c>
+      <c r="B93" s="29" t="str">
+        <f>'Hoja 1'!C93</f>
+        <v/>
+      </c>
+      <c r="C93" s="29" t="str">
+        <f>'Hoja 1'!D93</f>
+        <v/>
+      </c>
+      <c r="D93" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F93</f>
+        <v>+56</v>
+      </c>
+      <c r="E93" s="29" t="str">
+        <f>'Hoja 1'!E93</f>
+        <v/>
+      </c>
+      <c r="F93" s="29" t="str">
+        <f>'Hoja 1'!I93</f>
+        <v/>
+      </c>
       <c r="G93" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="94">
+      <c r="A94" s="29" t="str">
+        <f>'Hoja 1'!B94</f>
+        <v/>
+      </c>
+      <c r="B94" s="29" t="str">
+        <f>'Hoja 1'!C94</f>
+        <v/>
+      </c>
+      <c r="C94" s="29" t="str">
+        <f>'Hoja 1'!D94</f>
+        <v/>
+      </c>
+      <c r="D94" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F94</f>
+        <v>+56</v>
+      </c>
+      <c r="E94" s="29" t="str">
+        <f>'Hoja 1'!E94</f>
+        <v/>
+      </c>
+      <c r="F94" s="29" t="str">
+        <f>'Hoja 1'!I94</f>
+        <v/>
+      </c>
       <c r="G94" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="95">
+      <c r="A95" s="29" t="str">
+        <f>'Hoja 1'!B95</f>
+        <v/>
+      </c>
+      <c r="B95" s="29" t="str">
+        <f>'Hoja 1'!C95</f>
+        <v/>
+      </c>
+      <c r="C95" s="29" t="str">
+        <f>'Hoja 1'!D95</f>
+        <v/>
+      </c>
+      <c r="D95" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F95</f>
+        <v>+56</v>
+      </c>
+      <c r="E95" s="29" t="str">
+        <f>'Hoja 1'!E95</f>
+        <v/>
+      </c>
+      <c r="F95" s="29" t="str">
+        <f>'Hoja 1'!I95</f>
+        <v/>
+      </c>
       <c r="G95" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="96">
+      <c r="A96" s="29" t="str">
+        <f>'Hoja 1'!B96</f>
+        <v/>
+      </c>
+      <c r="B96" s="29" t="str">
+        <f>'Hoja 1'!C96</f>
+        <v/>
+      </c>
+      <c r="C96" s="29" t="str">
+        <f>'Hoja 1'!D96</f>
+        <v/>
+      </c>
+      <c r="D96" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F96</f>
+        <v>+56</v>
+      </c>
+      <c r="E96" s="29" t="str">
+        <f>'Hoja 1'!E96</f>
+        <v/>
+      </c>
+      <c r="F96" s="29" t="str">
+        <f>'Hoja 1'!I96</f>
+        <v/>
+      </c>
       <c r="G96" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="97">
+      <c r="A97" s="29" t="str">
+        <f>'Hoja 1'!B97</f>
+        <v/>
+      </c>
+      <c r="B97" s="29" t="str">
+        <f>'Hoja 1'!C97</f>
+        <v/>
+      </c>
+      <c r="C97" s="29" t="str">
+        <f>'Hoja 1'!D97</f>
+        <v/>
+      </c>
+      <c r="D97" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F97</f>
+        <v>+56</v>
+      </c>
+      <c r="E97" s="29" t="str">
+        <f>'Hoja 1'!E97</f>
+        <v/>
+      </c>
+      <c r="F97" s="29" t="str">
+        <f>'Hoja 1'!I97</f>
+        <v/>
+      </c>
       <c r="G97" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="98">
+      <c r="A98" s="29" t="str">
+        <f>'Hoja 1'!B98</f>
+        <v/>
+      </c>
+      <c r="B98" s="29" t="str">
+        <f>'Hoja 1'!C98</f>
+        <v/>
+      </c>
+      <c r="C98" s="29" t="str">
+        <f>'Hoja 1'!D98</f>
+        <v/>
+      </c>
+      <c r="D98" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F98</f>
+        <v>+56</v>
+      </c>
+      <c r="E98" s="29" t="str">
+        <f>'Hoja 1'!E98</f>
+        <v/>
+      </c>
+      <c r="F98" s="29" t="str">
+        <f>'Hoja 1'!I98</f>
+        <v/>
+      </c>
       <c r="G98" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="99">
+      <c r="A99" s="29" t="str">
+        <f>'Hoja 1'!B99</f>
+        <v/>
+      </c>
+      <c r="B99" s="29" t="str">
+        <f>'Hoja 1'!C99</f>
+        <v/>
+      </c>
+      <c r="C99" s="29" t="str">
+        <f>'Hoja 1'!D99</f>
+        <v/>
+      </c>
+      <c r="D99" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F99</f>
+        <v>+56</v>
+      </c>
+      <c r="E99" s="29" t="str">
+        <f>'Hoja 1'!E99</f>
+        <v/>
+      </c>
+      <c r="F99" s="29" t="str">
+        <f>'Hoja 1'!I99</f>
+        <v/>
+      </c>
       <c r="G99" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="100">
+      <c r="A100" s="29" t="str">
+        <f>'Hoja 1'!B100</f>
+        <v/>
+      </c>
+      <c r="B100" s="29" t="str">
+        <f>'Hoja 1'!C100</f>
+        <v/>
+      </c>
+      <c r="C100" s="29" t="str">
+        <f>'Hoja 1'!D100</f>
+        <v/>
+      </c>
+      <c r="D100" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F100</f>
+        <v>+56</v>
+      </c>
+      <c r="E100" s="29" t="str">
+        <f>'Hoja 1'!E100</f>
+        <v/>
+      </c>
+      <c r="F100" s="29" t="str">
+        <f>'Hoja 1'!I100</f>
+        <v/>
+      </c>
       <c r="G100" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="101">
+      <c r="A101" s="29" t="str">
+        <f>'Hoja 1'!B101</f>
+        <v/>
+      </c>
+      <c r="B101" s="29" t="str">
+        <f>'Hoja 1'!C101</f>
+        <v/>
+      </c>
+      <c r="C101" s="29" t="str">
+        <f>'Hoja 1'!D101</f>
+        <v/>
+      </c>
+      <c r="D101" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F101</f>
+        <v>+56</v>
+      </c>
+      <c r="E101" s="29" t="str">
+        <f>'Hoja 1'!E101</f>
+        <v/>
+      </c>
+      <c r="F101" s="29" t="str">
+        <f>'Hoja 1'!I101</f>
+        <v/>
+      </c>
       <c r="G101" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="102">
+      <c r="A102" s="29" t="str">
+        <f>'Hoja 1'!B102</f>
+        <v/>
+      </c>
+      <c r="B102" s="29" t="str">
+        <f>'Hoja 1'!C102</f>
+        <v/>
+      </c>
+      <c r="C102" s="29" t="str">
+        <f>'Hoja 1'!D102</f>
+        <v/>
+      </c>
+      <c r="D102" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F102</f>
+        <v>+56</v>
+      </c>
+      <c r="E102" s="29" t="str">
+        <f>'Hoja 1'!E102</f>
+        <v/>
+      </c>
+      <c r="F102" s="29" t="str">
+        <f>'Hoja 1'!I102</f>
+        <v/>
+      </c>
       <c r="G102" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="103">
+      <c r="A103" s="29" t="str">
+        <f>'Hoja 1'!B103</f>
+        <v/>
+      </c>
+      <c r="B103" s="29" t="str">
+        <f>'Hoja 1'!C103</f>
+        <v/>
+      </c>
+      <c r="C103" s="29" t="str">
+        <f>'Hoja 1'!D103</f>
+        <v/>
+      </c>
+      <c r="D103" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F103</f>
+        <v>+56</v>
+      </c>
+      <c r="E103" s="29" t="str">
+        <f>'Hoja 1'!E103</f>
+        <v/>
+      </c>
+      <c r="F103" s="29" t="str">
+        <f>'Hoja 1'!I103</f>
+        <v/>
+      </c>
       <c r="G103" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="104">
+      <c r="A104" s="29" t="str">
+        <f>'Hoja 1'!B104</f>
+        <v/>
+      </c>
+      <c r="B104" s="29" t="str">
+        <f>'Hoja 1'!C104</f>
+        <v/>
+      </c>
+      <c r="C104" s="29" t="str">
+        <f>'Hoja 1'!D104</f>
+        <v/>
+      </c>
+      <c r="D104" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F104</f>
+        <v>+56</v>
+      </c>
+      <c r="E104" s="29" t="str">
+        <f>'Hoja 1'!E104</f>
+        <v/>
+      </c>
+      <c r="F104" s="29" t="str">
+        <f>'Hoja 1'!I104</f>
+        <v/>
+      </c>
       <c r="G104" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="105">
+      <c r="A105" s="29" t="str">
+        <f>'Hoja 1'!B105</f>
+        <v/>
+      </c>
+      <c r="B105" s="29" t="str">
+        <f>'Hoja 1'!C105</f>
+        <v/>
+      </c>
+      <c r="C105" s="29" t="str">
+        <f>'Hoja 1'!D105</f>
+        <v/>
+      </c>
+      <c r="D105" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F105</f>
+        <v>+56</v>
+      </c>
+      <c r="E105" s="29" t="str">
+        <f>'Hoja 1'!E105</f>
+        <v/>
+      </c>
+      <c r="F105" s="29" t="str">
+        <f>'Hoja 1'!I105</f>
+        <v/>
+      </c>
       <c r="G105" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="106">
+      <c r="A106" s="29" t="str">
+        <f>'Hoja 1'!B106</f>
+        <v/>
+      </c>
+      <c r="B106" s="29" t="str">
+        <f>'Hoja 1'!C106</f>
+        <v/>
+      </c>
+      <c r="C106" s="29" t="str">
+        <f>'Hoja 1'!D106</f>
+        <v/>
+      </c>
+      <c r="D106" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F106</f>
+        <v>+56</v>
+      </c>
+      <c r="E106" s="29" t="str">
+        <f>'Hoja 1'!E106</f>
+        <v/>
+      </c>
+      <c r="F106" s="29" t="str">
+        <f>'Hoja 1'!I106</f>
+        <v/>
+      </c>
       <c r="G106" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="107">
+      <c r="A107" s="29" t="str">
+        <f>'Hoja 1'!B107</f>
+        <v/>
+      </c>
+      <c r="B107" s="29" t="str">
+        <f>'Hoja 1'!C107</f>
+        <v/>
+      </c>
+      <c r="C107" s="29" t="str">
+        <f>'Hoja 1'!D107</f>
+        <v/>
+      </c>
+      <c r="D107" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F107</f>
+        <v>+56</v>
+      </c>
+      <c r="E107" s="29" t="str">
+        <f>'Hoja 1'!E107</f>
+        <v/>
+      </c>
+      <c r="F107" s="29" t="str">
+        <f>'Hoja 1'!I107</f>
+        <v/>
+      </c>
       <c r="G107" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="108">
+      <c r="A108" s="29" t="str">
+        <f>'Hoja 1'!B108</f>
+        <v/>
+      </c>
+      <c r="B108" s="29" t="str">
+        <f>'Hoja 1'!C108</f>
+        <v/>
+      </c>
+      <c r="C108" s="29" t="str">
+        <f>'Hoja 1'!D108</f>
+        <v/>
+      </c>
+      <c r="D108" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F108</f>
+        <v>+56</v>
+      </c>
+      <c r="E108" s="29" t="str">
+        <f>'Hoja 1'!E108</f>
+        <v/>
+      </c>
+      <c r="F108" s="29" t="str">
+        <f>'Hoja 1'!I108</f>
+        <v/>
+      </c>
       <c r="G108" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="109">
+      <c r="A109" s="29" t="str">
+        <f>'Hoja 1'!B109</f>
+        <v/>
+      </c>
+      <c r="B109" s="29" t="str">
+        <f>'Hoja 1'!C109</f>
+        <v/>
+      </c>
+      <c r="C109" s="29" t="str">
+        <f>'Hoja 1'!D109</f>
+        <v/>
+      </c>
+      <c r="D109" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F109</f>
+        <v>+56</v>
+      </c>
+      <c r="E109" s="29" t="str">
+        <f>'Hoja 1'!E109</f>
+        <v/>
+      </c>
+      <c r="F109" s="29" t="str">
+        <f>'Hoja 1'!I109</f>
+        <v/>
+      </c>
       <c r="G109" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="110">
+      <c r="A110" s="29" t="str">
+        <f>'Hoja 1'!B110</f>
+        <v/>
+      </c>
+      <c r="B110" s="29" t="str">
+        <f>'Hoja 1'!C110</f>
+        <v/>
+      </c>
+      <c r="C110" s="29" t="str">
+        <f>'Hoja 1'!D110</f>
+        <v/>
+      </c>
+      <c r="D110" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F110</f>
+        <v>+56</v>
+      </c>
+      <c r="E110" s="29" t="str">
+        <f>'Hoja 1'!E110</f>
+        <v/>
+      </c>
+      <c r="F110" s="29" t="str">
+        <f>'Hoja 1'!I110</f>
+        <v/>
+      </c>
       <c r="G110" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="111">
+      <c r="A111" s="29" t="str">
+        <f>'Hoja 1'!B111</f>
+        <v/>
+      </c>
+      <c r="B111" s="29" t="str">
+        <f>'Hoja 1'!C111</f>
+        <v/>
+      </c>
+      <c r="C111" s="29" t="str">
+        <f>'Hoja 1'!D111</f>
+        <v/>
+      </c>
+      <c r="D111" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F111</f>
+        <v>+56</v>
+      </c>
+      <c r="E111" s="29" t="str">
+        <f>'Hoja 1'!E111</f>
+        <v/>
+      </c>
+      <c r="F111" s="29" t="str">
+        <f>'Hoja 1'!I111</f>
+        <v/>
+      </c>
       <c r="G111" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="112">
+      <c r="A112" s="29" t="str">
+        <f>'Hoja 1'!B112</f>
+        <v/>
+      </c>
+      <c r="B112" s="29" t="str">
+        <f>'Hoja 1'!C112</f>
+        <v/>
+      </c>
+      <c r="C112" s="29" t="str">
+        <f>'Hoja 1'!D112</f>
+        <v/>
+      </c>
+      <c r="D112" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F112</f>
+        <v>+56</v>
+      </c>
+      <c r="E112" s="29" t="str">
+        <f>'Hoja 1'!E112</f>
+        <v/>
+      </c>
+      <c r="F112" s="29" t="str">
+        <f>'Hoja 1'!I112</f>
+        <v/>
+      </c>
       <c r="G112" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="113">
+      <c r="A113" s="29" t="str">
+        <f>'Hoja 1'!B113</f>
+        <v/>
+      </c>
+      <c r="B113" s="29" t="str">
+        <f>'Hoja 1'!C113</f>
+        <v/>
+      </c>
+      <c r="C113" s="29" t="str">
+        <f>'Hoja 1'!D113</f>
+        <v/>
+      </c>
+      <c r="D113" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F113</f>
+        <v>+56</v>
+      </c>
+      <c r="E113" s="29" t="str">
+        <f>'Hoja 1'!E113</f>
+        <v/>
+      </c>
+      <c r="F113" s="29" t="str">
+        <f>'Hoja 1'!I113</f>
+        <v/>
+      </c>
       <c r="G113" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="114">
+      <c r="A114" s="29" t="str">
+        <f>'Hoja 1'!B114</f>
+        <v/>
+      </c>
+      <c r="B114" s="29" t="str">
+        <f>'Hoja 1'!C114</f>
+        <v/>
+      </c>
+      <c r="C114" s="29" t="str">
+        <f>'Hoja 1'!D114</f>
+        <v/>
+      </c>
+      <c r="D114" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F114</f>
+        <v>+56</v>
+      </c>
+      <c r="E114" s="29" t="str">
+        <f>'Hoja 1'!E114</f>
+        <v/>
+      </c>
+      <c r="F114" s="29" t="str">
+        <f>'Hoja 1'!I114</f>
+        <v/>
+      </c>
       <c r="G114" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="115">
+      <c r="A115" s="29" t="str">
+        <f>'Hoja 1'!B115</f>
+        <v/>
+      </c>
+      <c r="B115" s="29" t="str">
+        <f>'Hoja 1'!C115</f>
+        <v/>
+      </c>
+      <c r="C115" s="29" t="str">
+        <f>'Hoja 1'!D115</f>
+        <v/>
+      </c>
+      <c r="D115" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F115</f>
+        <v>+56</v>
+      </c>
+      <c r="E115" s="29" t="str">
+        <f>'Hoja 1'!E115</f>
+        <v/>
+      </c>
+      <c r="F115" s="29" t="str">
+        <f>'Hoja 1'!I115</f>
+        <v/>
+      </c>
       <c r="G115" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="116">
+      <c r="A116" s="29" t="str">
+        <f>'Hoja 1'!B116</f>
+        <v/>
+      </c>
+      <c r="B116" s="29" t="str">
+        <f>'Hoja 1'!C116</f>
+        <v/>
+      </c>
+      <c r="C116" s="29" t="str">
+        <f>'Hoja 1'!D116</f>
+        <v/>
+      </c>
+      <c r="D116" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F116</f>
+        <v>+56</v>
+      </c>
+      <c r="E116" s="29" t="str">
+        <f>'Hoja 1'!E116</f>
+        <v/>
+      </c>
+      <c r="F116" s="29" t="str">
+        <f>'Hoja 1'!I116</f>
+        <v/>
+      </c>
       <c r="G116" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="117">
+      <c r="A117" s="29" t="str">
+        <f>'Hoja 1'!B117</f>
+        <v/>
+      </c>
+      <c r="B117" s="29" t="str">
+        <f>'Hoja 1'!C117</f>
+        <v/>
+      </c>
+      <c r="C117" s="29" t="str">
+        <f>'Hoja 1'!D117</f>
+        <v/>
+      </c>
+      <c r="D117" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F117</f>
+        <v>+56</v>
+      </c>
+      <c r="E117" s="29" t="str">
+        <f>'Hoja 1'!E117</f>
+        <v/>
+      </c>
+      <c r="F117" s="29" t="str">
+        <f>'Hoja 1'!I117</f>
+        <v/>
+      </c>
       <c r="G117" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="118">
+      <c r="A118" s="29" t="str">
+        <f>'Hoja 1'!B118</f>
+        <v/>
+      </c>
+      <c r="B118" s="29" t="str">
+        <f>'Hoja 1'!C118</f>
+        <v/>
+      </c>
+      <c r="C118" s="29" t="str">
+        <f>'Hoja 1'!D118</f>
+        <v/>
+      </c>
+      <c r="D118" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F118</f>
+        <v>+56</v>
+      </c>
+      <c r="E118" s="29" t="str">
+        <f>'Hoja 1'!E118</f>
+        <v/>
+      </c>
+      <c r="F118" s="29" t="str">
+        <f>'Hoja 1'!I118</f>
+        <v/>
+      </c>
       <c r="G118" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="119">
+      <c r="A119" s="29" t="str">
+        <f>'Hoja 1'!B119</f>
+        <v/>
+      </c>
+      <c r="B119" s="29" t="str">
+        <f>'Hoja 1'!C119</f>
+        <v/>
+      </c>
+      <c r="C119" s="29" t="str">
+        <f>'Hoja 1'!D119</f>
+        <v/>
+      </c>
+      <c r="D119" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F119</f>
+        <v>+56</v>
+      </c>
+      <c r="E119" s="29" t="str">
+        <f>'Hoja 1'!E119</f>
+        <v/>
+      </c>
+      <c r="F119" s="29" t="str">
+        <f>'Hoja 1'!I119</f>
+        <v/>
+      </c>
       <c r="G119" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="120">
+      <c r="A120" s="29" t="str">
+        <f>'Hoja 1'!B120</f>
+        <v/>
+      </c>
+      <c r="B120" s="29" t="str">
+        <f>'Hoja 1'!C120</f>
+        <v/>
+      </c>
+      <c r="C120" s="29" t="str">
+        <f>'Hoja 1'!D120</f>
+        <v/>
+      </c>
+      <c r="D120" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F120</f>
+        <v>+56</v>
+      </c>
+      <c r="E120" s="29" t="str">
+        <f>'Hoja 1'!E120</f>
+        <v/>
+      </c>
+      <c r="F120" s="29" t="str">
+        <f>'Hoja 1'!I120</f>
+        <v/>
+      </c>
       <c r="G120" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="121">
+      <c r="A121" s="29" t="str">
+        <f>'Hoja 1'!B121</f>
+        <v/>
+      </c>
+      <c r="B121" s="29" t="str">
+        <f>'Hoja 1'!C121</f>
+        <v/>
+      </c>
+      <c r="C121" s="29" t="str">
+        <f>'Hoja 1'!D121</f>
+        <v/>
+      </c>
+      <c r="D121" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F121</f>
+        <v>+56</v>
+      </c>
+      <c r="E121" s="29" t="str">
+        <f>'Hoja 1'!E121</f>
+        <v/>
+      </c>
+      <c r="F121" s="29" t="str">
+        <f>'Hoja 1'!I121</f>
+        <v/>
+      </c>
       <c r="G121" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="122">
+      <c r="A122" s="29" t="str">
+        <f>'Hoja 1'!B122</f>
+        <v/>
+      </c>
+      <c r="B122" s="29" t="str">
+        <f>'Hoja 1'!C122</f>
+        <v/>
+      </c>
+      <c r="C122" s="29" t="str">
+        <f>'Hoja 1'!D122</f>
+        <v/>
+      </c>
+      <c r="D122" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F122</f>
+        <v>+56</v>
+      </c>
+      <c r="E122" s="29" t="str">
+        <f>'Hoja 1'!E122</f>
+        <v/>
+      </c>
+      <c r="F122" s="29" t="str">
+        <f>'Hoja 1'!I122</f>
+        <v/>
+      </c>
       <c r="G122" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="123">
+      <c r="A123" s="29" t="str">
+        <f>'Hoja 1'!B123</f>
+        <v/>
+      </c>
+      <c r="B123" s="29" t="str">
+        <f>'Hoja 1'!C123</f>
+        <v/>
+      </c>
+      <c r="C123" s="29" t="str">
+        <f>'Hoja 1'!D123</f>
+        <v/>
+      </c>
+      <c r="D123" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F123</f>
+        <v>+56</v>
+      </c>
+      <c r="E123" s="29" t="str">
+        <f>'Hoja 1'!E123</f>
+        <v/>
+      </c>
+      <c r="F123" s="29" t="str">
+        <f>'Hoja 1'!I123</f>
+        <v/>
+      </c>
       <c r="G123" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="124">
+      <c r="A124" s="29" t="str">
+        <f>'Hoja 1'!B124</f>
+        <v/>
+      </c>
+      <c r="B124" s="29" t="str">
+        <f>'Hoja 1'!C124</f>
+        <v/>
+      </c>
+      <c r="C124" s="29" t="str">
+        <f>'Hoja 1'!D124</f>
+        <v/>
+      </c>
+      <c r="D124" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F124</f>
+        <v>+56</v>
+      </c>
+      <c r="E124" s="29" t="str">
+        <f>'Hoja 1'!E124</f>
+        <v/>
+      </c>
+      <c r="F124" s="29" t="str">
+        <f>'Hoja 1'!I124</f>
+        <v/>
+      </c>
       <c r="G124" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="125">
+      <c r="A125" s="29" t="str">
+        <f>'Hoja 1'!B125</f>
+        <v/>
+      </c>
+      <c r="B125" s="29" t="str">
+        <f>'Hoja 1'!C125</f>
+        <v/>
+      </c>
+      <c r="C125" s="29" t="str">
+        <f>'Hoja 1'!D125</f>
+        <v/>
+      </c>
+      <c r="D125" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F125</f>
+        <v>+56</v>
+      </c>
+      <c r="E125" s="29" t="str">
+        <f>'Hoja 1'!E125</f>
+        <v/>
+      </c>
+      <c r="F125" s="29" t="str">
+        <f>'Hoja 1'!I125</f>
+        <v/>
+      </c>
       <c r="G125" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="126">
+      <c r="A126" s="29" t="str">
+        <f>'Hoja 1'!B126</f>
+        <v/>
+      </c>
+      <c r="B126" s="29" t="str">
+        <f>'Hoja 1'!C126</f>
+        <v/>
+      </c>
+      <c r="C126" s="29" t="str">
+        <f>'Hoja 1'!D126</f>
+        <v/>
+      </c>
+      <c r="D126" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F126</f>
+        <v>+56</v>
+      </c>
+      <c r="E126" s="29" t="str">
+        <f>'Hoja 1'!E126</f>
+        <v/>
+      </c>
+      <c r="F126" s="29" t="str">
+        <f>'Hoja 1'!I126</f>
+        <v/>
+      </c>
       <c r="G126" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="127">
+      <c r="A127" s="29" t="str">
+        <f>'Hoja 1'!B127</f>
+        <v/>
+      </c>
+      <c r="B127" s="29" t="str">
+        <f>'Hoja 1'!C127</f>
+        <v/>
+      </c>
+      <c r="C127" s="29" t="str">
+        <f>'Hoja 1'!D127</f>
+        <v/>
+      </c>
+      <c r="D127" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F127</f>
+        <v>+56</v>
+      </c>
+      <c r="E127" s="29" t="str">
+        <f>'Hoja 1'!E127</f>
+        <v/>
+      </c>
+      <c r="F127" s="29" t="str">
+        <f>'Hoja 1'!I127</f>
+        <v/>
+      </c>
       <c r="G127" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="128">
+      <c r="A128" s="29" t="str">
+        <f>'Hoja 1'!B128</f>
+        <v/>
+      </c>
+      <c r="B128" s="29" t="str">
+        <f>'Hoja 1'!C128</f>
+        <v/>
+      </c>
+      <c r="C128" s="29" t="str">
+        <f>'Hoja 1'!D128</f>
+        <v/>
+      </c>
+      <c r="D128" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F128</f>
+        <v>+56</v>
+      </c>
+      <c r="E128" s="29" t="str">
+        <f>'Hoja 1'!E128</f>
+        <v/>
+      </c>
+      <c r="F128" s="29" t="str">
+        <f>'Hoja 1'!I128</f>
+        <v/>
+      </c>
       <c r="G128" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="129">
+      <c r="A129" s="29" t="str">
+        <f>'Hoja 1'!B129</f>
+        <v/>
+      </c>
+      <c r="B129" s="29" t="str">
+        <f>'Hoja 1'!C129</f>
+        <v/>
+      </c>
+      <c r="C129" s="29" t="str">
+        <f>'Hoja 1'!D129</f>
+        <v/>
+      </c>
+      <c r="D129" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F129</f>
+        <v>+56</v>
+      </c>
+      <c r="E129" s="29" t="str">
+        <f>'Hoja 1'!E129</f>
+        <v/>
+      </c>
+      <c r="F129" s="29" t="str">
+        <f>'Hoja 1'!I129</f>
+        <v/>
+      </c>
       <c r="G129" s="22" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="130">
+      <c r="A130" s="29" t="str">
+        <f>'Hoja 1'!B130</f>
+        <v/>
+      </c>
+      <c r="B130" s="29" t="str">
+        <f>'Hoja 1'!C130</f>
+        <v/>
+      </c>
+      <c r="C130" s="29" t="str">
+        <f>'Hoja 1'!D130</f>
+        <v/>
+      </c>
+      <c r="D130" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F130</f>
+        <v>+56</v>
+      </c>
+      <c r="E130" s="29" t="str">
+        <f>'Hoja 1'!E130</f>
+        <v/>
+      </c>
+      <c r="F130" s="29" t="str">
+        <f>'Hoja 1'!I130</f>
+        <v/>
+      </c>
       <c r="G130" s="22" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="29" t="str">
+        <f>'Hoja 1'!B131</f>
+        <v/>
+      </c>
+      <c r="B131" s="29" t="str">
+        <f>'Hoja 1'!C131</f>
+        <v/>
+      </c>
+      <c r="C131" s="29" t="str">
+        <f>'Hoja 1'!D131</f>
+        <v/>
+      </c>
+      <c r="D131" s="29" t="str">
+        <f>"+56"&amp;'Hoja 1'!F131</f>
+        <v>+56</v>
+      </c>
+      <c r="E131" s="29" t="str">
+        <f>'Hoja 1'!E131</f>
+        <v/>
+      </c>
+      <c r="F131" s="29" t="str">
+        <f>'Hoja 1'!I131</f>
+        <v/>
+      </c>
+      <c r="G131" s="22" t="s">
         <v>334</v>
       </c>
     </row>

</xml_diff>